<commit_message>
STUD-60533 - Update StudioX templates
</commit_message>
<xml_diff>
--- a/CompleteWordTemplatefromExcelandEmail/contentFiles/any/any/pt0/VisualBasic/Project_Notebook.xlsx
+++ b/CompleteWordTemplatefromExcelandEmail/contentFiles/any/any/pt0/VisualBasic/Project_Notebook.xlsx
@@ -1,33 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\studio\Studio\UiPath.Studio.Plugin.Workflow\ProjectTemplates\Business Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\GitHub\Studio\Studio\UiPath.Studio.Plugin.Workflow\ProjectTemplates\Business Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B5E3D-CC52-4BC8-BE61-079C0D7486C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841250D0-30A1-4773-B3A3-B7E3E0F9044F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="18700" windowHeight="9580" activeTab="5" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
-    <sheet name="About the Project Notebook" sheetId="2" r:id="rId1"/>
+    <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
     <sheet name="Date" sheetId="1" r:id="rId2"/>
     <sheet name="Text" sheetId="3" r:id="rId3"/>
     <sheet name="Number" sheetId="4" r:id="rId4"/>
     <sheet name="File" sheetId="5" r:id="rId5"/>
-    <sheet name="Scratchpad" sheetId="6" r:id="rId6"/>
+    <sheet name="About the Project Notebook" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_A1">Scratchpad!$A$1</definedName>
+    <definedName name="_A2">Scratchpad!$A$2</definedName>
+    <definedName name="_A3">Scratchpad!$A$3</definedName>
     <definedName name="CleanNumber">Number!$B$5</definedName>
     <definedName name="Contains">Text!$B$13</definedName>
     <definedName name="Date_Input">Date!$B$4</definedName>
-    <definedName name="DatePlusDays">Date!$B$7</definedName>
-    <definedName name="DatePlusWorkingDays">Date!$B$8</definedName>
-    <definedName name="DateText">Date!$B$18</definedName>
-    <definedName name="Days">Date!$B$6</definedName>
+    <definedName name="DatePlusDays">Date!$B$8</definedName>
+    <definedName name="DatePlusWorkingDays">Date!$B$9</definedName>
+    <definedName name="DateText">Date!$B$19</definedName>
+    <definedName name="Days">Date!$B$7</definedName>
     <definedName name="FileExtension">File!$B$9</definedName>
     <definedName name="FileName">File!$B$8</definedName>
     <definedName name="FileNameNoExtension">File!$B$10</definedName>
@@ -35,30 +38,31 @@
     <definedName name="Folder">File!$B$11</definedName>
     <definedName name="FullFileName_Input">File!$B$6</definedName>
     <definedName name="Int">Number!$B$6</definedName>
-    <definedName name="LastMonthEndDate">Date!$C$13</definedName>
-    <definedName name="LastMonthStartDate">Date!$B$13</definedName>
+    <definedName name="LastMonthEndDate">Date!$C$14</definedName>
+    <definedName name="LastMonthStartDate">Date!$B$14</definedName>
     <definedName name="LastName">Text!$B$16</definedName>
-    <definedName name="LastWeekFriday">Date!$C$12</definedName>
-    <definedName name="LastWeekMonday">Date!$B$12</definedName>
-    <definedName name="LastWeekSunday">Date!$D$12</definedName>
+    <definedName name="LastWeekFriday">Date!$C$13</definedName>
+    <definedName name="LastWeekMonday">Date!$B$13</definedName>
+    <definedName name="LastWeekSunday">Date!$D$13</definedName>
     <definedName name="Length">Text!$B$6</definedName>
     <definedName name="LowerCase">Text!$B$8</definedName>
     <definedName name="Number_Input">Number!$B$4</definedName>
     <definedName name="NumberText_Input">Number!$B$11</definedName>
-    <definedName name="ReformattedDate">Date!$B$29</definedName>
+    <definedName name="preferred_date_format">Date!$B$6</definedName>
+    <definedName name="ReformattedDate">Date!$B$31</definedName>
     <definedName name="ReformattedFileName">File!$B$15</definedName>
     <definedName name="ReformattedNumber">Number!$B$15</definedName>
     <definedName name="Replace">Text!$B$11</definedName>
     <definedName name="Result">Text!$B$12</definedName>
     <definedName name="Search">Text!$B$10</definedName>
     <definedName name="Text_Input">Text!$B$4</definedName>
-    <definedName name="ThisMonthFirstWorkingDay">Date!$B$14</definedName>
-    <definedName name="ThisMonthLastWorkingDay">Date!$C$14</definedName>
-    <definedName name="Today">Date!$B$11</definedName>
+    <definedName name="ThisMonthFirstWorkingDay">Date!$B$15</definedName>
+    <definedName name="ThisMonthLastWorkingDay">Date!$C$15</definedName>
+    <definedName name="Today">Date!$B$12</definedName>
     <definedName name="Trimmed">Text!$B$5</definedName>
     <definedName name="TwoDecimals">Number!$B$7</definedName>
     <definedName name="UpperCase">Text!$B$7</definedName>
-    <definedName name="YYYYMMDD">Date!$B$9</definedName>
+    <definedName name="YYYYMMDD">Date!$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,30 +81,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -330,9 +312,6 @@
     <t xml:space="preserve">  - If you indicate a file name that doesn't exist, it will be created when you run your project.</t>
   </si>
   <si>
-    <t>Formulas for working with dates</t>
-  </si>
-  <si>
     <t>Formulas for working with text</t>
   </si>
   <si>
@@ -355,6 +334,19 @@
   </si>
   <si>
     <t>C:\temp\Untitled Document.docx</t>
+  </si>
+  <si>
+    <t>Preferred Format</t>
+  </si>
+  <si>
+    <t>yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Output Date Format</t>
+  </si>
+  <si>
+    <t>Formulas for working with dates
+Note: All dates are formatted using TEXT() to avoid formatting issues that can occur due to differences in formatting preferences</t>
   </si>
 </sst>
 </file>
@@ -820,7 +812,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -894,6 +886,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -914,6 +918,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1479,419 +1486,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="165.5546875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="30"/>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36"/>
-    </row>
-    <row r="2" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="D4" s="31"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53392D88-1157-4343-9701-AA198E0565D5}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="4" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="4" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-    </row>
-    <row r="2" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>43931</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
+        <v>44097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B7" s="25">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+    <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="2">
-        <f ca="1">Date_Input+Days</f>
-        <v>43938</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="B8" s="43" t="str">
+        <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
+        <v>2020-09-30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="2">
-        <f ca="1">WORKDAY(Date_Input, Days)</f>
-        <v>43942</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" s="43" t="str">
+        <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
+        <v>2020-10-02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B10" s="44" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20200410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+        <v>20200923</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2">
-        <f ca="1">TODAY()</f>
-        <v>43931</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" s="43" t="str">
+        <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
+        <v>2020-09-23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2">
-        <f ca="1">TODAY()-WEEKDAY(TODAY(),2)-6</f>
-        <v>43920</v>
-      </c>
-      <c r="C12" s="2">
-        <f ca="1">LastWeekMonday+4</f>
-        <v>43924</v>
-      </c>
-      <c r="D12" s="2">
-        <f ca="1">LastWeekFriday+2</f>
-        <v>43926</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" s="43" t="str">
+        <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
+        <v>2020-09-14</v>
+      </c>
+      <c r="C13" s="43" t="str">
+        <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
+        <v>2020-09-18</v>
+      </c>
+      <c r="D13" s="45" t="str">
+        <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
+        <v>2020-09-20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2">
-        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1)</f>
-        <v>43891</v>
-      </c>
-      <c r="C13" s="2">
-        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY()), 0)</f>
-        <v>43921</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" s="43" t="str">
+        <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
+        <v>2020-08-01</v>
+      </c>
+      <c r="C14" s="43" t="str">
+        <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
+        <v>2020-08-31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2">
-        <f ca="1">WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1)</f>
-        <v>43922</v>
-      </c>
-      <c r="C14" s="2">
-        <f ca="1">WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1)</f>
-        <v>43951</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="45" t="s">
+      <c r="B15" s="43" t="str">
+        <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
+        <v>2020-09-01</v>
+      </c>
+      <c r="C15" s="43" t="str">
+        <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
+        <v>2020-09-30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B19" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="6" t="str">
-        <f>LEFT(B18, FIND(B19, B18)-1)</f>
+      <c r="B23" s="6" t="str">
+        <f>LEFT(B19, FIND(B20, B19)-1)</f>
         <v>2008</v>
       </c>
-      <c r="C22" s="6" t="str">
-        <f>RIGHT(B18, LEN(B18)-LEN(B22)-1)</f>
+      <c r="C23" s="6" t="str">
+        <f>RIGHT(B19, LEN(B19)-LEN(B23)-1)</f>
         <v>12月31日 (水)</v>
       </c>
-      <c r="D22" s="7" t="str">
-        <f>IF(D19&lt;&gt;"", LEFT(C22, FIND(D19, C22)-1), C22)</f>
+      <c r="D23" s="7" t="str">
+        <f>IF(D20&lt;&gt;"", LEFT(C23, FIND(D20, C23)-1), C23)</f>
         <v>12月31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="6" t="str">
-        <f>LEFT(C22, FIND(C19, C22)-1)</f>
+      <c r="B24" s="6" t="str">
+        <f>LEFT(C23, FIND(C20, C23)-1)</f>
         <v>12</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="6" t="str">
-        <f>RIGHT(D22, LEN(D22)-LEN(B23)-1)</f>
-        <v>31</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="6" t="str">
+        <f>RIGHT(D23, LEN(D23)-LEN(B24)-1)</f>
         <v>31</v>
-      </c>
-      <c r="B25" s="6" t="str" cm="1">
-        <f t="array" ref="B25">_xlfn.SWITCH(FIND("Y", B20), 1, B22, 2, B23, 3, B24)</f>
-        <v>2008</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="6" t="str" cm="1">
-        <f t="array" ref="B26">_xlfn.SWITCH(FIND("M", B20), 1, B22, 2, B23, 3, B24)</f>
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f>IF(FIND("Y", B21) = 1, B23, IF(FIND("Y", B21) = 2, B24, B25))</f>
+        <v>2008</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <f>FIND("Y", B21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="6" t="str" cm="1">
-        <f t="array" ref="B27">_xlfn.SWITCH(FIND("D", B20), 1, B22, 2, B23, 3, B24)</f>
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B27" s="6" t="str">
+        <f>IF(FIND("M", B21) = 1, B23, IF(FIND("M", B21) = 2, B24, B25))</f>
+        <v>12</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="6"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6" t="str">
+        <f>IF(FIND("D", B21) = 1, B23, IF(FIND("D", B21) = 2, B24, B25))</f>
+        <v>31</v>
+      </c>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="6" t="str">
+        <f>preferred_date_format</f>
+        <v>yyyy-mm-dd</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="8">
-        <f>DATE(B25, B26, B27)</f>
-        <v>39813</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="B31" s="8" t="str">
+        <f>TEXT(DATE(B26, B27, B28), B30)</f>
+        <v>2008-12-31</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A17:D17"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
   </mergeCells>
@@ -1908,36 +1831,36 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="25" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1957,7 +1880,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1979,7 +1902,7 @@
         <v>C.</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1999,7 +1922,7 @@
         <v>C. Doe</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2019,7 +1942,7 @@
         <v>John C.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -2039,7 +1962,7 @@
         <v>Doe</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>64</v>
       </c>
@@ -2048,7 +1971,7 @@
         <v>John C. Doe</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2059,7 +1982,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2070,7 +1993,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2082,24 +2005,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="b">
-        <f>IF(IFERROR(FIND(B10, Text), FALSE), TRUE, FALSE)</f>
-        <v>0</v>
+        <f>IF(IFERROR(FIND(B10,_xlfn.SINGLE( Text_Input)), FALSE), TRUE, FALSE)</f>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2111,7 +2034,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2123,7 +2046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>64</v>
       </c>
@@ -2146,37 +2069,37 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="49"/>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="53"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2184,7 +2107,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>68</v>
       </c>
@@ -2193,7 +2116,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2202,7 +2125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -2211,20 +2134,20 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="45" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="47"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -2232,7 +2155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
@@ -2241,7 +2164,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>35</v>
       </c>
@@ -2249,13 +2172,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>36</v>
       </c>
@@ -2283,62 +2206,62 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="4" width="15.109375" customWidth="1"/>
+    <col min="3" max="4" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="48"/>
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="52"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="49"/>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="53"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="47"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="51"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="26"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="17"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>40</v>
       </c>
@@ -2347,7 +2270,7 @@
         <v>Untitled Document.docx</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>42</v>
       </c>
@@ -2356,7 +2279,7 @@
         <v>docx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>41</v>
       </c>
@@ -2365,7 +2288,7 @@
         <v>Untitled Document</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="24" t="s">
         <v>56</v>
       </c>
@@ -2374,7 +2297,7 @@
         <v>C:\temp\</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>57</v>
       </c>
@@ -2394,17 +2317,128 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="165.54296875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="30"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36"/>
+    </row>
+    <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="35"/>
+      <c r="D4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="35"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="35"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="35"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="35"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="35"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="35"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="35"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="35"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="35"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="35"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="35"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="35"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>